<commit_message>
Revert "Lagged DV Created"
This reverts commit bd22904c50e8dea9b6e669356b752e94cffcad2d.
</commit_message>
<xml_diff>
--- a/Control Data/COVID-19_Regional_Safety_Assessment.xlsx
+++ b/Control Data/COVID-19_Regional_Safety_Assessment.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chacr\OneDrive\Documents\Coding\JHU Data\COVID-19\Control Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19" documentId="8_{F6F706B0-5678-4720-A996-9156B59A44D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D14AFFBB-58EF-4555-BCB8-AB9D2A744C5C}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="8_{F6F706B0-5678-4720-A996-9156B59A44D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{70570444-0F44-4091-B218-79763C18456B}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="COVID-19_Regional_Safety_Assess" sheetId="1" r:id="rId1"/>
@@ -843,10 +843,10 @@
     <t>Location:</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.dkv.global/covid-safety-assessment-250-list </t>
+  </si>
+  <si>
     <t>Taiwan</t>
-  </si>
-  <si>
-    <t>https://ourworldindata.org/future-population-growth</t>
   </si>
 </sst>
 </file>
@@ -1704,7 +1704,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I253"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -2160,7 +2160,7 @@
         <v>11</v>
       </c>
       <c r="B16" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="C16">
         <v>132.94</v>
@@ -9071,8 +9071,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9094,11 +9094,14 @@
         <v>268</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>